<commit_message>
Add kpi_salary to contract (#351)
</commit_message>
<xml_diff>
--- a/apps/hrm/fixtures/import_templates/contract_appendix_template.xlsx
+++ b/apps/hrm/fixtures/import_templates/contract_appendix_template.xlsx
@@ -39,12 +39,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="004472C4"/>
-        <bgColor rgb="004472C4"/>
+        <fgColor rgb="004F81BD"/>
+        <bgColor rgb="004F81BD"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -52,13 +52,19 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -426,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,90 +443,135 @@
     <col width="10" customWidth="1" min="1" max="1"/>
     <col width="15" customWidth="1" min="2" max="2"/>
     <col width="20" customWidth="1" min="3" max="3"/>
-    <col width="15" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
     <col width="15" customWidth="1" min="5" max="5"/>
     <col width="15" customWidth="1" min="6" max="6"/>
-    <col width="40" customWidth="1" min="7" max="7"/>
-    <col width="30" customWidth="1" min="8" max="8"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
+    <col width="15" customWidth="1" min="8" max="8"/>
+    <col width="15" customWidth="1" min="9" max="9"/>
+    <col width="15" customWidth="1" min="10" max="10"/>
+    <col width="15" customWidth="1" min="11" max="11"/>
+    <col width="40" customWidth="1" min="12" max="12"/>
+    <col width="30" customWidth="1" min="13" max="13"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Số Thứ Tự</t>
+          <t>Số thứ tự</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Mã Nhân Viên</t>
+          <t>Mã nhân viên</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Số Hợp Đồng</t>
+          <t>Số hợp đồng</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Số Phụ Lục</t>
+          <t>Số phụ lục</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Ngày Ký</t>
+          <t>Ngày ký</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Ngày Hiệu Lực</t>
+          <t>Ngày hiệu lực</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Nội Dung Thay Đổi</t>
+          <t>Lương cơ bản</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Ghi Chú</t>
+          <t>Lương KPI</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Phụ cấp ăn trưa</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Phụ cấp điện thoại</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Phụ cấp khác</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Nội dung thay đổi</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Ghi chú</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="B2" t="n">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>NV001</t>
+        </is>
+      </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>MV000001</t>
+          <t>123/2025/HD-MVL</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>01/2024/HD-MVL</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr"/>
+          <t>01/2025/PLHD-MVL</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>01/01/2025</t>
+        </is>
+      </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-01-15</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>2025-02-01</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Salary adjustment from 15,000,000 to 18,000,000</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>Approved by HR Manager</t>
-        </is>
-      </c>
+          <t>01/01/2025</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>10000000</v>
+      </c>
+      <c r="H2" t="n">
+        <v>5000000</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="J2" t="n">
+        <v>500000</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Điều chỉnh lương</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>